<commit_message>
Se añaden lineas  para los tres armonicos principales
</commit_message>
<xml_diff>
--- a/Transformdas_a.xlsx
+++ b/Transformdas_a.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Frecuencia Maxima alcanzada</t>
+          <t>Frecuencia del primer armonico</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Frecuencia del segundo armonico</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Frecuencia tercer armonico</t>
         </is>
       </c>
     </row>
@@ -455,7 +465,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>141.2991939307726</v>
+        <v>141.2991939307731</v>
+      </c>
+      <c r="D2" t="n">
+        <v>847.7951635846375</v>
+      </c>
+      <c r="E2" t="n">
+        <v>707.4442863916547</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +484,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>126.7848101265822</v>
+        <v>127.5949367088606</v>
+      </c>
+      <c r="D3" t="n">
+        <v>632.3037974683548</v>
+      </c>
+      <c r="E3" t="n">
+        <v>778.9367088607596</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +503,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>119.8338071287994</v>
+        <v>119.8338071287999</v>
+      </c>
+      <c r="D4" t="n">
+        <v>719.877542094905</v>
+      </c>
+      <c r="E4" t="n">
+        <v>239.6676142575989</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +522,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>129.6950240770466</v>
+        <v>130.5510968432318</v>
+      </c>
+      <c r="D5" t="n">
+        <v>257.2498662386306</v>
+      </c>
+      <c r="E5" t="n">
+        <v>781.1663991439273</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +541,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>772.4119706678994</v>
+        <v>772.9404769769444</v>
+      </c>
+      <c r="D6" t="n">
+        <v>128.1627799431863</v>
+      </c>
+      <c r="E6" t="n">
+        <v>889.2118649666377</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +560,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>574.246159681396</v>
+        <v>575.763322586763</v>
+      </c>
+      <c r="D7" t="n">
+        <v>768.4430115683672</v>
+      </c>
+      <c r="E7" t="n">
+        <v>384.6007965105255</v>
       </c>
     </row>
     <row r="8">
@@ -535,6 +581,12 @@
       <c r="C8" t="n">
         <v>721.4938418752481</v>
       </c>
+      <c r="D8" t="n">
+        <v>538.7365911799761</v>
+      </c>
+      <c r="E8" t="n">
+        <v>180.3734604688125</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -546,7 +598,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>760.1137109118745</v>
+        <v>760.113710911874</v>
+      </c>
+      <c r="D9" t="n">
+        <v>607.0413295429698</v>
+      </c>
+      <c r="E9" t="n">
+        <v>912.3113929586707</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +617,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>962.1611950979518</v>
+        <v>962.8768226138291</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1285.624832274801</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1126.03989623401</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +636,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>284.394366197183</v>
+        <v>285.2957746478878</v>
+      </c>
+      <c r="D11" t="n">
+        <v>568.3380281690143</v>
+      </c>
+      <c r="E11" t="n">
+        <v>856.788732394366</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +655,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>173.0811045879541</v>
+        <v>174.8206131767774</v>
+      </c>
+      <c r="D12" t="n">
+        <v>348.771472059143</v>
+      </c>
+      <c r="E12" t="n">
+        <v>693.1941726462278</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +674,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>637.3207660683847</v>
+        <v>638.122931916173</v>
+      </c>
+      <c r="D13" t="n">
+        <v>160.0320866339116</v>
+      </c>
+      <c r="E13" t="n">
+        <v>478.4919282061569</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +693,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>157.7424023154849</v>
+        <v>157.7424023154845</v>
+      </c>
+      <c r="D14" t="n">
+        <v>315.4848046309698</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1420.40520984081</v>
       </c>
     </row>
     <row r="15">
@@ -626,6 +714,12 @@
       <c r="C15" t="n">
         <v>147.1032745591938</v>
       </c>
+      <c r="D15" t="n">
+        <v>293.1989924433246</v>
+      </c>
+      <c r="E15" t="n">
+        <v>442.3173803526447</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -637,7 +731,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>159.4117647058824</v>
+        <v>159.4117647058829</v>
+      </c>
+      <c r="D16" t="n">
+        <v>320</v>
+      </c>
+      <c r="E16" t="n">
+        <v>480</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +750,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>327.7443846883898</v>
+        <v>326.9007697985871</v>
+      </c>
+      <c r="D17" t="n">
+        <v>164.0830960666458</v>
+      </c>
+      <c r="E17" t="n">
+        <v>491.4056733101334</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +769,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>149.2472179794895</v>
+        <v>149.2472179794891</v>
+      </c>
+      <c r="D18" t="n">
+        <v>305.4767619463237</v>
+      </c>
+      <c r="E18" t="n">
+        <v>453.8511891773951</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +788,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>619.9973927779947</v>
+        <v>619.9973927779956</v>
+      </c>
+      <c r="D19" t="n">
+        <v>153.8260982922693</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1239.99478555599</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +807,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>303.8829487900957</v>
+        <v>304.5260873060533</v>
+      </c>
+      <c r="D20" t="n">
+        <v>606.8011898062546</v>
+      </c>
+      <c r="E20" t="n">
+        <v>150.8159819921211</v>
       </c>
     </row>
     <row r="21">
@@ -704,6 +828,12 @@
       <c r="C21" t="n">
         <v>162.9268292682927</v>
       </c>
+      <c r="D21" t="n">
+        <v>648.7804878048782</v>
+      </c>
+      <c r="E21" t="n">
+        <v>486.8292682926831</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -715,7 +845,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>192.2869955156953</v>
+        <v>192.2869955156948</v>
+      </c>
+      <c r="D22" t="n">
+        <v>383.1390134529147</v>
+      </c>
+      <c r="E22" t="n">
+        <v>766.2780269058298</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +864,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1376.100628930818</v>
+        <v>1376.100628930817</v>
+      </c>
+      <c r="D23" t="n">
+        <v>124.9475890985323</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1490.146750524109</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +883,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>126.5474552957357</v>
+        <v>125.900153734121</v>
+      </c>
+      <c r="D24" t="n">
+        <v>252.7712598106641</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1276.155028724007</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +902,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1455.863995720145</v>
+        <v>1456.339535160198</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1361.707186589788</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1531.950306128515</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +921,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1175.153889199776</v>
+        <v>1174.656469564136</v>
+      </c>
+      <c r="D26" t="n">
+        <v>131.5674936268106</v>
+      </c>
+      <c r="E26" t="n">
+        <v>393.7076416091522</v>
       </c>
     </row>
     <row r="27">
@@ -782,6 +942,12 @@
       <c r="C27" t="n">
         <v>166.0675772825307</v>
       </c>
+      <c r="D27" t="n">
+        <v>661.3946800862686</v>
+      </c>
+      <c r="E27" t="n">
+        <v>332.1351545650614</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -795,6 +961,12 @@
       <c r="C28" t="n">
         <v>1422.323635672181</v>
       </c>
+      <c r="D28" t="n">
+        <v>850.3517779045451</v>
+      </c>
+      <c r="E28" t="n">
+        <v>994.8659440958359</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -806,7 +978,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1316.692667706709</v>
+        <v>1316.692667706708</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1170.046801872075</v>
+      </c>
+      <c r="E29" t="n">
+        <v>732.6053042121684</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +997,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1427.764326069411</v>
+        <v>1427.76432606941</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1319.612590799032</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1049.233252623083</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +1016,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>315.6547703682636</v>
+        <v>316.792265036258</v>
+      </c>
+      <c r="D31" t="n">
+        <v>159.8180008531217</v>
+      </c>
+      <c r="E31" t="n">
+        <v>791.1275415896489</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +1035,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>225.4143646408843</v>
+        <v>227.1823204419888</v>
+      </c>
+      <c r="D32" t="n">
+        <v>449.9447513812156</v>
+      </c>
+      <c r="E32" t="n">
+        <v>678.0110497237565</v>
       </c>
     </row>
     <row r="33">
@@ -860,6 +1056,12 @@
       <c r="C33" t="n">
         <v>246.8429830831546</v>
       </c>
+      <c r="D33" t="n">
+        <v>1729.807005003574</v>
+      </c>
+      <c r="E33" t="n">
+        <v>494.639027877055</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -871,7 +1073,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1551.517387694862</v>
+        <v>1552.255326999354</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1032.746056636841</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1293.23863112259</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +1092,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>248.4276729559751</v>
+        <v>248.4276729559747</v>
+      </c>
+      <c r="D35" t="n">
+        <v>494.7589098532499</v>
+      </c>
+      <c r="E35" t="n">
+        <v>743.1865828092241</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +1111,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>971.0910786446998</v>
+        <v>971.0910786447002</v>
+      </c>
+      <c r="D36" t="n">
+        <v>728.6291576002486</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1458.501709667393</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +1130,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>462.4980009595397</v>
+        <v>463.77738685431</v>
+      </c>
+      <c r="D37" t="n">
+        <v>694.0668479130018</v>
+      </c>
+      <c r="E37" t="n">
+        <v>233.4879257956181</v>
       </c>
     </row>
     <row r="38">
@@ -925,6 +1151,12 @@
       <c r="C38" t="n">
         <v>668.3221000354733</v>
       </c>
+      <c r="D38" t="n">
+        <v>222.7740333451579</v>
+      </c>
+      <c r="E38" t="n">
+        <v>445.5480666903159</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -936,7 +1168,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>708.2018927444797</v>
+        <v>708.2018927444788</v>
+      </c>
+      <c r="D39" t="n">
+        <v>176.1303890641429</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1240.273396424815</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +1187,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>180.58757902566</v>
+        <v>181.182595760506</v>
+      </c>
+      <c r="D40" t="n">
+        <v>359.6876162142062</v>
+      </c>
+      <c r="E40" t="n">
+        <v>541.167720342135</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +1206,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>173.7147201368434</v>
+        <v>172.9544806614081</v>
+      </c>
+      <c r="D41" t="n">
+        <v>346.289081060534</v>
+      </c>
+      <c r="E41" t="n">
+        <v>520.3839209350945</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +1225,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>783.5842362642634</v>
+        <v>782.8171445009111</v>
+      </c>
+      <c r="D42" t="n">
+        <v>263.4960207114773</v>
+      </c>
+      <c r="E42" t="n">
+        <v>522.7730367245176</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +1244,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>273.0348258706467</v>
+        <v>273.0348258706472</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1095.323383084577</v>
+      </c>
+      <c r="E43" t="n">
+        <v>548.4577114427866</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1263,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>908.0004066280371</v>
+        <v>907.1871505540307</v>
+      </c>
+      <c r="D44" t="n">
+        <v>226.4918166107554</v>
+      </c>
+      <c r="E44" t="n">
+        <v>681.1019619802782</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1282,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>177.335229966809</v>
+        <v>177.3352299668086</v>
+      </c>
+      <c r="D45" t="n">
+        <v>350.8771929824561</v>
+      </c>
+      <c r="E45" t="n">
+        <v>700.806069227122</v>
       </c>
     </row>
     <row r="46">
@@ -1029,6 +1303,12 @@
       <c r="C46" t="n">
         <v>293.4455802766088</v>
       </c>
+      <c r="D46" t="n">
+        <v>584.4858689116054</v>
+      </c>
+      <c r="E46" t="n">
+        <v>877.9314491882142</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1042,6 +1322,12 @@
       <c r="C47" t="n">
         <v>1069.073783359498</v>
       </c>
+      <c r="D47" t="n">
+        <v>802.9827315541602</v>
+      </c>
+      <c r="E47" t="n">
+        <v>534.5368916797488</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1053,7 +1339,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>281.3303769401336</v>
+        <v>280.620842572062</v>
+      </c>
+      <c r="D48" t="n">
+        <v>841.1529933481161</v>
+      </c>
+      <c r="E48" t="n">
+        <v>562.3059866962312</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1358,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>841.1236210622083</v>
+        <v>842.0334356874791</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1122.25634027067</v>
+      </c>
+      <c r="E49" t="n">
+        <v>560.9007164790173</v>
       </c>
     </row>
     <row r="50">
@@ -1081,6 +1379,12 @@
       <c r="C50" t="n">
         <v>801.0645375914837</v>
       </c>
+      <c r="D50" t="n">
+        <v>199.6007984031939</v>
+      </c>
+      <c r="E50" t="n">
+        <v>398.5362608117102</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1094,6 +1398,12 @@
       <c r="C51" t="n">
         <v>187.5945537065054</v>
       </c>
+      <c r="D51" t="n">
+        <v>375.8614893259373</v>
+      </c>
+      <c r="E51" t="n">
+        <v>747.6886871743145</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1107,6 +1417,12 @@
       <c r="C52" t="n">
         <v>198.4196663740122</v>
       </c>
+      <c r="D52" t="n">
+        <v>398.0099502487565</v>
+      </c>
+      <c r="E52" t="n">
+        <v>801.287679250805</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1118,7 +1434,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>813.3844895905399</v>
+        <v>813.8876658909367</v>
+      </c>
+      <c r="D53" t="n">
+        <v>203.534813510284</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1023.209006855777</v>
       </c>
     </row>
     <row r="54">
@@ -1132,6 +1454,12 @@
       </c>
       <c r="C54" t="n">
         <v>205.5563552612639</v>
+      </c>
+      <c r="D54" t="n">
+        <v>822.8012091550308</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1028.357564416295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>